<commit_message>
New graphs for paper
</commit_message>
<xml_diff>
--- a/exercises/basic/evaluation/digest-stats.xlsx
+++ b/exercises/basic/evaluation/digest-stats.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacknorris/Desktop/Coding/p4-tutorials/exercises/basic/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BA44947-67E0-224D-B746-501FA8928010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674C68FA-E922-AE48-A922-74996B6FB31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{71BE2E1C-4152-8C43-AC4A-C542B382FE49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{71BE2E1C-4152-8C43-AC4A-C542B382FE49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
   <si>
     <t>﻿ANALOG:</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>MAX</t>
+  </si>
+  <si>
+    <t>Missing Data Rate (%)</t>
+  </si>
+  <si>
+    <t>Standard Deviation of Approximation Error Measurments</t>
+  </si>
+  <si>
+    <t>Angle error</t>
+  </si>
+  <si>
+    <t>Missing Data Rate %</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89AD914-E462-0244-9CC9-0454910C5635}">
-  <dimension ref="A2:H51"/>
+  <dimension ref="A2:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,10 +1021,13 @@
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="43.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="52.6640625" customWidth="1"/>
+    <col min="13" max="13" width="24.83203125" customWidth="1"/>
+    <col min="16" max="16" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1038,8 +1053,23 @@
         <f ca="1">AVERAGE(F:F)</f>
         <v>1.0036963399999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M2" t="s">
+        <v>107</v>
+      </c>
+      <c r="P2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1065,8 +1095,23 @@
         <f ca="1">STDEV(F:F)</f>
         <v>4.8503888150900933E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.113078736087662</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>4.2039797521405999E-2</v>
+      </c>
+      <c r="Q3">
+        <v>0.113078736087662</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1092,8 +1137,23 @@
         <f ca="1">MIN(F:F)</f>
         <v>1.000945</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>0.13565881390919601</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>5.7580257926705E-2</v>
+      </c>
+      <c r="Q4">
+        <v>0.13565881390919601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1119,8 +1179,23 @@
         <f ca="1">MAX(F:F)</f>
         <v>1.0324120000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>0.15592321466704101</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>6.6301403203123693E-2</v>
+      </c>
+      <c r="Q5">
+        <v>0.15592321466704101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1139,8 +1214,23 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.001482</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>0.17173736161074399</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>5.37841045228254E-2</v>
+      </c>
+      <c r="Q6">
+        <v>0.17173736161074399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1159,8 +1249,23 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.0029939999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>0.156188257688813</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>6.9592245651760795E-2</v>
+      </c>
+      <c r="Q7">
+        <v>0.156188257688813</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1179,8 +1284,23 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.0014419999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>0.163128550795407</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>8.3470828106687905E-2</v>
+      </c>
+      <c r="Q8">
+        <v>0.163128550795407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1199,8 +1319,23 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.0021850000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>0.207387696126413</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>8.3833530230314701E-2</v>
+      </c>
+      <c r="Q9">
+        <v>0.207387696126413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1219,8 +1354,23 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.005479</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>0.45668498876458802</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>0.15468930185714899</v>
+      </c>
+      <c r="Q10">
+        <v>0.45668498876458802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1239,8 +1389,23 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.00373</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>0.43974896833390598</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>0.16920721323379501</v>
+      </c>
+      <c r="Q11">
+        <v>0.43974896833390598</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1259,8 +1424,23 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.003395</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>0.28274015118616802</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>0.62769374040992398</v>
+      </c>
+      <c r="Q12">
+        <v>0.28274015118616802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1280,7 +1460,7 @@
         <v>1.0025170000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1300,7 +1480,7 @@
         <v>1.002267</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1320,7 +1500,7 @@
         <v>1.0010680000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>

</xml_diff>